<commit_message>
No code changes detected; skipping commit.
</commit_message>
<xml_diff>
--- a/backend/src/data/Costi_ingredienti.xlsx
+++ b/backend/src/data/Costi_ingredienti.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>ingredienti</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>piume</t>
+  </si>
+  <si>
+    <t>vetro</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1130,9 @@
       <c r="M30" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A31" s="4"/>
+      <c r="A31" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="B31" s="11"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>

</xml_diff>